<commit_message>
Add next few test methods for login negative paths
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/UsersData.xlsx
+++ b/src/test/java/TestData/UsersData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4abb4d561aa445b3/Desktop/Testing/Java_kursSelenium_testelka/DataDrivenTestingProject/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{DA5DFF2A-CB1C-499B-BD91-9DA0352DA9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25432882-8239-42BC-BB74-4101DB579B7C}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{DA5DFF2A-CB1C-499B-BD91-9DA0352DA9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85F6C9FF-893B-4325-8A2B-E9A507B43235}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{11F1207F-42B7-49FD-A6A4-AE0A40BC7628}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{11F1207F-42B7-49FD-A6A4-AE0A40BC7628}"/>
   </bookViews>
   <sheets>
-    <sheet name="UserCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="UsernameCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="UserEmailCredentials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>pass1</t>
   </si>
@@ -39,9 +40,6 @@
     <t>pass4</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -91,13 +89,49 @@
   </si>
   <si>
     <t>Coookie</t>
+  </si>
+  <si>
+    <t>Vendetta@test1.com</t>
+  </si>
+  <si>
+    <t>Ashen@test2.com</t>
+  </si>
+  <si>
+    <t>Porto@test3.com</t>
+  </si>
+  <si>
+    <t>beautiful_Antonia@test4.com</t>
+  </si>
+  <si>
+    <t>Armstrong@test5.com</t>
+  </si>
+  <si>
+    <t>spaceX@test6.com</t>
+  </si>
+  <si>
+    <t>agulek@test7.com</t>
+  </si>
+  <si>
+    <t>wild_baby@test8.com</t>
+  </si>
+  <si>
+    <t>greasy-muffin@test9.com</t>
+  </si>
+  <si>
+    <t>Coookie@test10.com</t>
+  </si>
+  <si>
+    <t>User email</t>
+  </si>
+  <si>
+    <t>User name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +149,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,14 +179,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -181,6 +226,18 @@
 </file>
 
 <file path=xl/persons/person12.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person13.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person14.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person15.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -515,27 +572,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227DA9AF-185A-4916-9AEC-8B0A11C66994}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -543,7 +600,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -551,7 +608,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -559,7 +616,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -567,50 +624,50 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -618,4 +675,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3284A69F-66E7-4ACE-B29B-432F51B92EE1}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7BBF43F5-D64F-404A-9AB0-4BBAD8A4B70B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{27D1AA69-543C-4921-8062-4205F6AAE3F5}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{6C2A1C8B-5BC6-4EFB-A756-2E1B38A34113}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{E53934E4-56EB-4573-9FD6-A66E88099460}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{1F6F2CFD-B0CC-48D6-AC5E-FD621A8E8C50}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{97F36356-8607-4B9D-BC36-79932326F6A3}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{27418592-9EE7-4BE6-B3DE-6B168A28B7CC}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{93A31A09-2A15-477F-9F35-78CA2E293ADC}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{0619BBA2-31CD-4AD2-8827-922F6A744C9A}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{6DD915A8-BDF8-441E-B266-C847AE1FEB8D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>